<commit_message>
Updated the tests for the new fixtures. Refactored the upload code so that it puts files against a resource and checks the digest of uploaded files one at a time.
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA96EBB4-6AA4-7B44-9B06-DD770B292236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8746F5DA-3E87-8B49-9BF4-93F75DC60340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9060" yWindow="5600" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3240" yWindow="2600" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Recipe</t>
   </si>
@@ -45,9 +45,6 @@
     <t>Dataset</t>
   </si>
   <si>
-    <t>SubjectId</t>
-  </si>
-  <si>
     <t>YYYY</t>
   </si>
   <si>
@@ -63,12 +60,6 @@
     <t>Configuration</t>
   </si>
   <si>
-    <t>{SubjectName}-{SubjectId}</t>
-  </si>
-  <si>
-    <t>{YYYY}{MM}{DD}-{Label}.dcm</t>
-  </si>
-  <si>
     <t>Mappings</t>
   </si>
   <si>
@@ -91,6 +82,21 @@
   </si>
   <si>
     <t>Paths</t>
+  </si>
+  <si>
+    <t>{SubjectName}-{ID}</t>
+  </si>
+  <si>
+    <t>{YYYY}{MM}{DD}</t>
+  </si>
+  <si>
+    <t>{Label}</t>
+  </si>
+  <si>
+    <t>{filename}.dcm</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -462,10 +468,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68FE643B-0B72-8E46-99FC-7188AD10E0D6}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -475,75 +481,81 @@
     <col min="3" max="3" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
         <v>8</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C12" s="2" t="s">
         <v>17</v>
-      </c>
-      <c r="C11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed test_config.py to work with the new config for basic
</commit_message>
<xml_diff>
--- a/tests/fixtures/template.xlsx
+++ b/tests/fixtures/template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mike/working/xnat-uploader/tests/fixtures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8746F5DA-3E87-8B49-9BF4-93F75DC60340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E7C477B-B4EA-314A-B1EB-3606F42C60BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3240" yWindow="2600" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15880" yWindow="7060" windowWidth="29340" windowHeight="15200" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="23">
   <si>
     <t>Recipe</t>
   </si>
@@ -45,18 +45,6 @@
     <t>Dataset</t>
   </si>
   <si>
-    <t>YYYY</t>
-  </si>
-  <si>
-    <t>MM</t>
-  </si>
-  <si>
-    <t>DD</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
     <t>Configuration</t>
   </si>
   <si>
@@ -87,16 +75,22 @@
     <t>{SubjectName}-{ID}</t>
   </si>
   <si>
-    <t>{YYYY}{MM}{DD}</t>
-  </si>
-  <si>
-    <t>{Label}</t>
-  </si>
-  <si>
     <t>{filename}.dcm</t>
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>**</t>
+  </si>
+  <si>
+    <t>{Directory}</t>
+  </si>
+  <si>
+    <t>DICOM:StudyDate</t>
+  </si>
+  <si>
+    <t>Directory</t>
   </si>
 </sst>
 </file>
@@ -483,38 +477,38 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>22</v>
-      </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -522,13 +516,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -536,26 +524,26 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>